<commit_message>
Tinkering with Garden City folder and trying to get a generalized extraction procedure to work.
</commit_message>
<xml_diff>
--- a/control/test.xlsx
+++ b/control/test.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+  <si>
+    <t>Filename</t>
+  </si>
   <si>
     <t>Audit Observation</t>
   </si>
@@ -28,28 +31,13 @@
     <t>Management_x000D_Action</t>
   </si>
   <si>
-    <t>Status of_x000D_Implementa_x000D_tion</t>
-  </si>
-  <si>
-    <t>Reasons for_x000D_partial/Non_x000D_Implementati_x000D_on</t>
-  </si>
-  <si>
     <t>Status of_x000D_Implementation</t>
   </si>
   <si>
     <t>Reasons for partial/Non_x000D_Implementation</t>
   </si>
   <si>
-    <t>1.    At end of audit period the Accountant had not yet updated the books of_x000D_accounts,  and have  posted only the  transactions up to  June  30,  2009,  in_x000D_effect this office has not received the Post-Closing Trial Balance within the_x000D_required period as prescribed in Section 72 of the NGAs Volume I resulting_x000D_to the delay in its verification by the COA.</t>
-  </si>
-  <si>
-    <t>2.The Accountant failed to submit to the Auditor the liquidation_x000D_reports  of  the  accountable  officers  within  grace  period,  in_x000D_violation of COA Circular No.97-002 dated February 7, 2007,_x000D_hence the necessary audit of the disbursements allegedly spent_x000D_for  development  projects  and  procurement  of  vehicles  and_x000D_equipments was not undertaken.</t>
-  </si>
-  <si>
-    <t>3.The accuracy and validity of the balance of the Property, Plant_x000D_and Equipment and Inventory accounts totalling 161,884,690.99_x000D_was  not  ascertained  due  to  the  failure  of  the  General  Service_x000D_Office  (GSO)  and  concerned  offices  to  submit  Report  on  the_x000D_Physical Count of Property, Plant and Equipment (RPCPPE) and_x000D_Inventory for 2009 on the prescribed period.</t>
-  </si>
-  <si>
-    <t>4Purchase Orders,  contracts and reports on the acceptance and_x000D_deliveries of supplies and materials were not submitted to the_x000D_Auditor within the prescribed period mandated under Paragraph_x000D_A. COA circular No. 96-010 dated August 16, 1996, preventing_x000D_the conduct of review of the contract and communicating to the_x000D_management the defects, or non-compliance thereto.</t>
+    <t>../data/unzipped/02-LamitanCity2010_Status_of_Prior_Years_Audit_Recommendations.pdf</t>
   </si>
   <si>
     <t>5.The LGU appropriated a total amount of_x000D_P1,896,000.00 for GAD related activities or_x000D_1.21% of the total estimated Internal Revenue_x000D_Allocation  of  P230,000,000.00  instead  of_x000D_P11,500,000.00 or 5% of the total estimated_x000D_IRA as mandated under the Joint Circular No_x000D_2004-001 dated April 5, 2004._x000D__x000D_.</t>
@@ -58,49 +46,16 @@
     <t>During the year 2009, the LGU planned to undertake_x000D_Social Reform Agenda (SRA)- Flagship Project with a_x000D_budget  of  P  10,300,000.00  of  which  P  10,125,797.31_x000D_was spent during the year, but the LGU did not submit_x000D_documents  justifying  the  program,  thus  we  have  not_x000D_verified the results of the program.</t>
   </si>
   <si>
-    <t>The City Mayor shall require the OIC City_x000D_Accountant to submit these trial balances in accordance with_x000D_the  provisions  of  Section  72  of  the  New  Government_x000D_Accounting System (NGAS) Volume I in order to facilitate_x000D_the  immediate  verification  and  submission  to  the  GAFMIS_x000D_considering that the deadline set had been overdue.</t>
-  </si>
-  <si>
-    <t>We recommend that the City Mayor shall direct the_x000D_accountant  to  submit  the  liquidation  reports  of  the_x000D_Accountable  Officers  to  the  Office  of  the  Auditor_x000D_immediately  pursuant  to  COA  Circular  No.  97-002,_x000D_andeffectthecorrectionintheFSastothe_x000D_unliquidated cash Advances.</t>
-  </si>
-  <si>
-    <t>Itisrecommendedthatthelocalofficial_x000D_concernedshouldsubmittheyearendPhysical_x000D_Inventory Report of PPE within the prescribed period_x000D_to give the team ample time to validate its correctness.</t>
-  </si>
-  <si>
-    <t>It is recommended that the concerned agency officials to_x000D_submit to the Auditor, within five (5) days from issuance, the_x000D_copies of the purchase orders or contracts and acceptance and_x000D_inspection report with the necessary data and information to_x000D_avoid confusion and delay in the confirmation of deliveries.</t>
-  </si>
-  <si>
     <t>We  recommend  that  5%  of  the  total  IRA  be_x000D_appropriated for Gender  and Development  (GAD) Fund,_x000D_independent  and  separate  from such  other  fund  such  as_x000D_20% DF, and expended in accordance with the programs</t>
   </si>
   <si>
     <t>We recommend that the City Mayor shall encourage the_x000D_Accountant and concerned Official to submit the necessary_x000D_document as above discussed</t>
   </si>
   <si>
-    <t>Page 13 and 14_x000D_CY 2009 AAR</t>
-  </si>
-  <si>
-    <t>Page 14 and 15_x000D_CY 2009 AAR</t>
-  </si>
-  <si>
-    <t>Page 15 and 16_x000D_CY 2009 AAR</t>
-  </si>
-  <si>
-    <t>Page 16-18_x000D_CY 2009 AAR</t>
-  </si>
-  <si>
     <t>Page 18 and_x000D_19_x000D_CY 2009 AAR</t>
   </si>
   <si>
     <t>Page 19_x000D_CY 2009 AAR</t>
-  </si>
-  <si>
-    <t>Implemented</t>
-  </si>
-  <si>
-    <t>implemented</t>
-  </si>
-  <si>
-    <t>Unimplemented_x000D_Reiterated in_x000D_Part II</t>
   </si>
   <si>
     <t>Unimplemented</t>
@@ -461,13 +416,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -489,110 +444,45 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>26</v>
-      </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" t="s">
-        <v>29</v>
+      <c r="G3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>